<commit_message>
SQL files + maj BDD
</commit_message>
<xml_diff>
--- a/BDD.xlsx
+++ b/BDD.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentmounier/IUT/TUTS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reiko\Documents\Cours\Stage\TUTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14145" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>TABLE USERS</t>
   </si>
@@ -86,12 +86,6 @@
     <t>PROJET</t>
   </si>
   <si>
-    <t>DOMAINE_ACT</t>
-  </si>
-  <si>
-    <t>VALID_CHARTE</t>
-  </si>
-  <si>
     <t>OFFRE</t>
   </si>
   <si>
@@ -144,6 +138,33 @@
   </si>
   <si>
     <t>CONNAISSANCE</t>
+  </si>
+  <si>
+    <t>VALIDATION</t>
+  </si>
+  <si>
+    <t>a filtrer</t>
+  </si>
+  <si>
+    <t>ACT_ID</t>
+  </si>
+  <si>
+    <t>DOMAINE_ACTION</t>
+  </si>
+  <si>
+    <t>ID_DA</t>
+  </si>
+  <si>
+    <t>ACT1</t>
+  </si>
+  <si>
+    <t>ACT2</t>
+  </si>
+  <si>
+    <t>ACT3</t>
+  </si>
+  <si>
+    <t>ACT4</t>
   </si>
 </sst>
 </file>
@@ -190,6 +211,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -458,26 +482,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="2" width="14.625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="12" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" customWidth="1"/>
+    <col min="4" max="12" width="14.625" customWidth="1"/>
+    <col min="17" max="17" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -527,119 +551,149 @@
         <v>19</v>
       </c>
       <c r="Q2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="R2" t="s">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G14" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="H14" t="s">
         <v>37</v>
       </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" t="s">
-        <v>39</v>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>